<commit_message>
Failed site download bug
</commit_message>
<xml_diff>
--- a/failed_tests.xlsx
+++ b/failed_tests.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,81 +448,217 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>districtdetails.com</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>401</v>
+          <t>boroughexpedition.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>401</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>boroughbulletin.com</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>401</v>
+          <t>communitynavigate.com</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>401</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>localelinker.com</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>401</v>
+          <t>communityprobe.com</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>401</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>areaamplifier.com</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>401</v>
+          <t>communitypilots.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>401</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>metromecca.com</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>403</v>
+          <t>districtexplorer.com</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>401</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>localelookup.com</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>401</v>
+          <t>localeguided.com</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>localelively.com</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>401</v>
+          <t>communityroamers.com</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>401</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>metromeander.com</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>401</v>
+          <t>communitytrackers.com</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>401</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>localequest.xyz</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>districtsearchers.com</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>401</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>localequest.com</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>metropathfinders.com</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>401</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>regionaldetective.com</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>regionalprobes.com</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>regionalscavenger.com</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>townrovers.com</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>401</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>townsleuth.com</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>401</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>vicinityfinders.com</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>401</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>